<commit_message>
alter sql & built environmen
</commit_message>
<xml_diff>
--- a/環境構築/環境構築手順書(インポート ~MySQL).xlsx
+++ b/環境構築/環境構築手順書(インポート ~MySQL).xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenta\OneDrive\ドキュメント\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenta\0519git\Document\環境構築\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="目次" sheetId="3" r:id="rId1"/>
     <sheet name="1-1プロジェクトのインポート" sheetId="1" r:id="rId2"/>
     <sheet name="1-2eclipse サーバ作成" sheetId="2" r:id="rId3"/>
-    <sheet name="2-1XAMPPのインストール" sheetId="4" r:id="rId4"/>
+    <sheet name="2-1Mysqlのインストール" sheetId="4" r:id="rId4"/>
     <sheet name="2-2テーブルの構築" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t xml:space="preserve">「tomcat-users.xml」のソースコード中の&lt;tomcat-users&gt;タグの一行下に以下の設定を追記する。  </t>
   </si>
@@ -43,36 +43,6 @@
     <t>2.サーバの作成　14ステップ</t>
     <rPh sb="6" eb="8">
       <t>サクセイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>http://techacademy.jp/magazine/1722</t>
-  </si>
-  <si>
-    <t>http://techacademy.jp/magazine/4137</t>
-  </si>
-  <si>
-    <t>3.XAMPPのインストール　設定</t>
-    <rPh sb="15" eb="17">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・XAMPP自体のインストール</t>
-    <rPh sb="6" eb="8">
-      <t>ジタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・MySQLの設定等</t>
-    <rPh sb="7" eb="9">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>トウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -107,10 +77,6 @@
     <rPh sb="4" eb="6">
       <t>サクセイ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>XAMPPのインストール</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -386,6 +352,24 @@
     <rPh sb="34" eb="36">
       <t>ソウテイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mysqlのインストール</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://webkaru.net/mysql/install-windows/</t>
+  </si>
+  <si>
+    <t>2-1.Mysqlのインストール　設定</t>
+    <rPh sb="17" eb="19">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mysqlのインストール</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -628,8 +612,36 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3940,27 +3952,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:W10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="2" spans="3:23" x14ac:dyDescent="0.15">
       <c r="C2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="3:23" x14ac:dyDescent="0.15">
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
       <c r="H4" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -3980,14 +3992,14 @@
     </row>
     <row r="5" spans="3:23" x14ac:dyDescent="0.15">
       <c r="C5" s="12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="14"/>
       <c r="H5" s="12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
@@ -4007,14 +4019,14 @@
     </row>
     <row r="6" spans="3:23" x14ac:dyDescent="0.15">
       <c r="C6" s="15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
       <c r="H6" s="15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
@@ -4034,14 +4046,14 @@
     </row>
     <row r="7" spans="3:23" x14ac:dyDescent="0.15">
       <c r="C7" s="18" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="20"/>
       <c r="H7" s="18" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
@@ -4061,14 +4073,14 @@
     </row>
     <row r="8" spans="3:23" x14ac:dyDescent="0.15">
       <c r="C8" s="21" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
       <c r="H8" s="21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
@@ -4142,7 +4154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:U184"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
@@ -4150,7 +4162,7 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C4" s="24" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.15">
@@ -4160,7 +4172,7 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="21:21" x14ac:dyDescent="0.15">
@@ -4175,17 +4187,17 @@
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C44" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C79" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C114" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="2:3" ht="14.25" x14ac:dyDescent="0.15">
@@ -4193,12 +4205,12 @@
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C149" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="184" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C184" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -4226,52 +4238,52 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C44" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C79" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C114" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C150" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C185" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="220" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C220" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="255" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C255" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="290" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C290" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="325" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C325" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="326" spans="3:4" x14ac:dyDescent="0.15">
@@ -4281,32 +4293,32 @@
     </row>
     <row r="362" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C362" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="397" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C397" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="433" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C433" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="469" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C469" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="505" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C505" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="506" spans="3:4" x14ac:dyDescent="0.15">
       <c r="D506" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -4318,10 +4330,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:F12"/>
+  <dimension ref="B6:F10"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AK20" sqref="A1:XFD1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
@@ -4331,32 +4343,22 @@
   <sheetData>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B6" s="11" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.15">
       <c r="C8" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.15">
       <c r="E9" s="11" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
       <c r="F10" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E11" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="F12" s="11" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -4371,19 +4373,19 @@
   <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>